<commit_message>
Add LOO test script and update output filenames
Renamed Speech_completo_test.py to Speech_test_loo.py and updated the output filename in the script to reflect LOO (Leave-One-Out) testing. Added a new SLURM batch script Speech_test_loo.sh to run the updated Python script. Updated the speech_rfe.xlsx results file.
</commit_message>
<xml_diff>
--- a/Results/speech_rfe.xlsx
+++ b/Results/speech_rfe.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -840,501 +840,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>10%</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>RF</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>{'max_depth': None, 'min_samples_leaf': 1, 'min_samples_split': 10, 'n_estimators': 40}</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>['duration_a', 'jitter_ddp_a', 'hnr_max_a', 'f2_std_a', 'f3_std_a', 'f3_max_a', 'mfcc_4_a', 'mfcc_5_a', 'mfcc_11_a', 'f0_std_e', 'shimmer_apq5_e', 'shimmer_apq11_e', 'hnr_std_e', 'hnr_max_e', 'f1_std_e', 'f1_max_e', 'mfcc_5_e', 'mfcc_11_e', 'f3_mean_i', 'f3_min_i', 'mfcc_6_i', 'f1_min_o', 'f2_min_o', 'mfcc_4_o', 'mfcc_7_o', 'jitter_rap_u', 'jitter_ddp_u', 'hnr_min_u', 'f3_mean_u', 'mfcc_9_u', 'f0_median_k', 'jitter_local_absolute_k', 'f1_max_k', 'f2_min_k', 'mfcc_6_k', 'mfcc_11_k', 'EnergyBurst_k', 'tot_articulation_p', 'shimmer_apq11_p', 'f2_max_p', 'mfcc_1_p', 'mfcc_10_p', 'tot_articulation_t', 'mfcc_1_t', 'mfcc_3_t']</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>6</v>
-      </c>
-      <c r="F8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" t="n">
-        <v>8</v>
-      </c>
-      <c r="H8" t="n">
-        <v>4</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="O8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>10%</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>XGB</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>{'learning_rate': 0.1, 'max_depth': 2, 'n_estimators': 200, 'subsample': 0.5}</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>['duration_a', 'jitter_ddp_a', 'hnr_max_a', 'f2_std_a', 'f3_std_a', 'f3_max_a', 'mfcc_4_a', 'mfcc_5_a', 'mfcc_11_a', 'f0_std_e', 'shimmer_apq5_e', 'shimmer_apq11_e', 'hnr_std_e', 'hnr_max_e', 'f1_std_e', 'f1_max_e', 'mfcc_5_e', 'mfcc_11_e', 'f3_mean_i', 'f3_min_i', 'mfcc_6_i', 'f1_min_o', 'f2_min_o', 'mfcc_4_o', 'mfcc_7_o', 'jitter_rap_u', 'jitter_ddp_u', 'hnr_min_u', 'f3_mean_u', 'mfcc_9_u', 'f0_median_k', 'jitter_local_absolute_k', 'f1_max_k', 'f2_min_k', 'mfcc_6_k', 'mfcc_11_k', 'EnergyBurst_k', 'tot_articulation_p', 'shimmer_apq11_p', 'f2_max_p', 'mfcc_1_p', 'mfcc_10_p', 'tot_articulation_t', 'mfcc_1_t', 'mfcc_3_t']</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>7</v>
-      </c>
-      <c r="F9" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" t="n">
-        <v>8</v>
-      </c>
-      <c r="H9" t="n">
-        <v>3</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.7368421052631579</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.7777777777777778</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="O9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>10%</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>KNN</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>{'metric': 'euclidean', 'n_neighbors': 5, 'weights': 'uniform'}</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>['duration_a', 'jitter_ddp_a', 'hnr_max_a', 'f2_std_a', 'f3_std_a', 'f3_max_a', 'mfcc_4_a', 'mfcc_5_a', 'mfcc_11_a', 'f0_std_e', 'shimmer_apq5_e', 'shimmer_apq11_e', 'hnr_std_e', 'hnr_max_e', 'f1_std_e', 'f1_max_e', 'mfcc_5_e', 'mfcc_11_e', 'f3_mean_i', 'f3_min_i', 'mfcc_6_i', 'f1_min_o', 'f2_min_o', 'mfcc_4_o', 'mfcc_7_o', 'jitter_rap_u', 'jitter_ddp_u', 'hnr_min_u', 'f3_mean_u', 'mfcc_9_u', 'f0_median_k', 'jitter_local_absolute_k', 'f1_max_k', 'f2_min_k', 'mfcc_6_k', 'mfcc_11_k', 'EnergyBurst_k', 'tot_articulation_p', 'shimmer_apq11_p', 'f2_max_p', 'mfcc_1_p', 'mfcc_10_p', 'tot_articulation_t', 'mfcc_1_t', 'mfcc_3_t']</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>6</v>
-      </c>
-      <c r="F10" t="n">
-        <v>4</v>
-      </c>
-      <c r="G10" t="n">
-        <v>6</v>
-      </c>
-      <c r="H10" t="n">
-        <v>4</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0.918918918918919</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>10%</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>MLP</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>{'activation': 'relu', 'alpha': 0.0001, 'hidden_layer_sizes': (64, 32), 'learning_rate': 'constant'}</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>['duration_a', 'jitter_ddp_a', 'hnr_max_a', 'f2_std_a', 'f3_std_a', 'f3_max_a', 'mfcc_4_a', 'mfcc_5_a', 'mfcc_11_a', 'f0_std_e', 'shimmer_apq5_e', 'shimmer_apq11_e', 'hnr_std_e', 'hnr_max_e', 'f1_std_e', 'f1_max_e', 'mfcc_5_e', 'mfcc_11_e', 'f3_mean_i', 'f3_min_i', 'mfcc_6_i', 'f1_min_o', 'f2_min_o', 'mfcc_4_o', 'mfcc_7_o', 'jitter_rap_u', 'jitter_ddp_u', 'hnr_min_u', 'f3_mean_u', 'mfcc_9_u', 'f0_median_k', 'jitter_local_absolute_k', 'f1_max_k', 'f2_min_k', 'mfcc_6_k', 'mfcc_11_k', 'EnergyBurst_k', 'tot_articulation_p', 'shimmer_apq11_p', 'f2_max_p', 'mfcc_1_p', 'mfcc_10_p', 'tot_articulation_t', 'mfcc_1_t', 'mfcc_3_t']</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>5</v>
-      </c>
-      <c r="F11" t="n">
-        <v>4</v>
-      </c>
-      <c r="G11" t="n">
-        <v>6</v>
-      </c>
-      <c r="H11" t="n">
-        <v>5</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.5263157894736842</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.5555555555555556</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0.9333333333333333</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>SVM</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>{'C': 0.1, 'degree': 2, 'gamma': 0.0001, 'kernel': 'linear'}</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>['duration_a', 'jitter_ddp_a', 'hnr_max_a', 'f2_std_a', 'f3_std_a', 'f3_max_a', 'mfcc_4_a', 'mfcc_5_a', 'mfcc_11_a', 'f0_std_e', 'shimmer_apq5_e', 'shimmer_apq11_e', 'hnr_std_e', 'hnr_max_e', 'f1_std_e', 'f1_max_e', 'mfcc_5_e', 'mfcc_11_e', 'f3_mean_i', 'f3_min_i', 'mfcc_6_i', 'f1_min_o', 'f2_min_o', 'mfcc_4_o', 'mfcc_7_o', 'f0_std_u', 'jitter_local_u', 'jitter_rap_u', 'jitter_ddp_u', 'hnr_min_u', 'cpp_u', 'f3_mean_u', 'mfcc_6_u', 'mfcc_9_u', 'duration_k', 'f0_median_k', 'f0_75_k', 'jitter_local_absolute_k', 'f2_median_k', 'f1_max_k', 'f2_min_k', 'mfcc_6_k', 'mfcc_11_k', 'EnergyBurst_k', 'tot_articulation_p', 'shimmer_apq11_p', 'f2_max_p', 'mfcc_1_p', 'mfcc_10_p', 'mfcc_11_p', 'tot_articulation_t', 'mfcc_1_t', 'mfcc_3_t', 'mfcc_6_t', 'HFLFRatio_t']</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>5</v>
-      </c>
-      <c r="F12" t="n">
-        <v>3</v>
-      </c>
-      <c r="G12" t="n">
-        <v>7</v>
-      </c>
-      <c r="H12" t="n">
-        <v>5</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.5555555555555556</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="O12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>RF</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>{'max_depth': None, 'min_samples_leaf': 2, 'min_samples_split': 10, 'n_estimators': 20}</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>['duration_a', 'jitter_ddp_a', 'hnr_max_a', 'f2_std_a', 'f3_std_a', 'f3_max_a', 'mfcc_4_a', 'mfcc_5_a', 'mfcc_11_a', 'f0_std_e', 'shimmer_apq5_e', 'shimmer_apq11_e', 'hnr_std_e', 'hnr_max_e', 'f1_std_e', 'f1_max_e', 'mfcc_5_e', 'mfcc_11_e', 'f3_mean_i', 'f3_min_i', 'mfcc_6_i', 'f1_min_o', 'f2_min_o', 'mfcc_4_o', 'mfcc_7_o', 'f0_std_u', 'jitter_local_u', 'jitter_rap_u', 'jitter_ddp_u', 'hnr_min_u', 'cpp_u', 'f3_mean_u', 'mfcc_6_u', 'mfcc_9_u', 'duration_k', 'f0_median_k', 'f0_75_k', 'jitter_local_absolute_k', 'f2_median_k', 'f1_max_k', 'f2_min_k', 'mfcc_6_k', 'mfcc_11_k', 'EnergyBurst_k', 'tot_articulation_p', 'shimmer_apq11_p', 'f2_max_p', 'mfcc_1_p', 'mfcc_10_p', 'mfcc_11_p', 'tot_articulation_t', 'mfcc_1_t', 'mfcc_3_t', 'mfcc_6_t', 'HFLFRatio_t']</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>7</v>
-      </c>
-      <c r="F13" t="n">
-        <v>2</v>
-      </c>
-      <c r="G13" t="n">
-        <v>8</v>
-      </c>
-      <c r="H13" t="n">
-        <v>3</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0.7368421052631579</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0.7777777777777778</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0.9866666666666667</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>XGB</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>{'learning_rate': 0.1, 'max_depth': 2, 'n_estimators': 200, 'subsample': 0.3}</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>['duration_a', 'jitter_ddp_a', 'hnr_max_a', 'f2_std_a', 'f3_std_a', 'f3_max_a', 'mfcc_4_a', 'mfcc_5_a', 'mfcc_11_a', 'f0_std_e', 'shimmer_apq5_e', 'shimmer_apq11_e', 'hnr_std_e', 'hnr_max_e', 'f1_std_e', 'f1_max_e', 'mfcc_5_e', 'mfcc_11_e', 'f3_mean_i', 'f3_min_i', 'mfcc_6_i', 'f1_min_o', 'f2_min_o', 'mfcc_4_o', 'mfcc_7_o', 'f0_std_u', 'jitter_local_u', 'jitter_rap_u', 'jitter_ddp_u', 'hnr_min_u', 'cpp_u', 'f3_mean_u', 'mfcc_6_u', 'mfcc_9_u', 'duration_k', 'f0_median_k', 'f0_75_k', 'jitter_local_absolute_k', 'f2_median_k', 'f1_max_k', 'f2_min_k', 'mfcc_6_k', 'mfcc_11_k', 'EnergyBurst_k', 'tot_articulation_p', 'shimmer_apq11_p', 'f2_max_p', 'mfcc_1_p', 'mfcc_10_p', 'mfcc_11_p', 'tot_articulation_t', 'mfcc_1_t', 'mfcc_3_t', 'mfcc_6_t', 'HFLFRatio_t']</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>8</v>
-      </c>
-      <c r="F14" t="n">
-        <v>2</v>
-      </c>
-      <c r="G14" t="n">
-        <v>8</v>
-      </c>
-      <c r="H14" t="n">
-        <v>2</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="O14" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>KNN</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>{'metric': 'manhattan', 'n_neighbors': 15, 'weights': 'uniform'}</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>['duration_a', 'jitter_ddp_a', 'hnr_max_a', 'f2_std_a', 'f3_std_a', 'f3_max_a', 'mfcc_4_a', 'mfcc_5_a', 'mfcc_11_a', 'f0_std_e', 'shimmer_apq5_e', 'shimmer_apq11_e', 'hnr_std_e', 'hnr_max_e', 'f1_std_e', 'f1_max_e', 'mfcc_5_e', 'mfcc_11_e', 'f3_mean_i', 'f3_min_i', 'mfcc_6_i', 'f1_min_o', 'f2_min_o', 'mfcc_4_o', 'mfcc_7_o', 'f0_std_u', 'jitter_local_u', 'jitter_rap_u', 'jitter_ddp_u', 'hnr_min_u', 'cpp_u', 'f3_mean_u', 'mfcc_6_u', 'mfcc_9_u', 'duration_k', 'f0_median_k', 'f0_75_k', 'jitter_local_absolute_k', 'f2_median_k', 'f1_max_k', 'f2_min_k', 'mfcc_6_k', 'mfcc_11_k', 'EnergyBurst_k', 'tot_articulation_p', 'shimmer_apq11_p', 'f2_max_p', 'mfcc_1_p', 'mfcc_10_p', 'mfcc_11_p', 'tot_articulation_t', 'mfcc_1_t', 'mfcc_3_t', 'mfcc_6_t', 'HFLFRatio_t']</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>5</v>
-      </c>
-      <c r="F15" t="n">
-        <v>2</v>
-      </c>
-      <c r="G15" t="n">
-        <v>8</v>
-      </c>
-      <c r="H15" t="n">
-        <v>5</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0.5882352941176471</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="N15" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="O15" t="n">
-        <v>0.7733333333333333</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>MLP</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>{'activation': 'tanh', 'alpha': 0.0001, 'hidden_layer_sizes': (16, 8), 'learning_rate': 'constant'}</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>['duration_a', 'jitter_ddp_a', 'hnr_max_a', 'f2_std_a', 'f3_std_a', 'f3_max_a', 'mfcc_4_a', 'mfcc_5_a', 'mfcc_11_a', 'f0_std_e', 'shimmer_apq5_e', 'shimmer_apq11_e', 'hnr_std_e', 'hnr_max_e', 'f1_std_e', 'f1_max_e', 'mfcc_5_e', 'mfcc_11_e', 'f3_mean_i', 'f3_min_i', 'mfcc_6_i', 'f1_min_o', 'f2_min_o', 'mfcc_4_o', 'mfcc_7_o', 'f0_std_u', 'jitter_local_u', 'jitter_rap_u', 'jitter_ddp_u', 'hnr_min_u', 'cpp_u', 'f3_mean_u', 'mfcc_6_u', 'mfcc_9_u', 'duration_k', 'f0_median_k', 'f0_75_k', 'jitter_local_absolute_k', 'f2_median_k', 'f1_max_k', 'f2_min_k', 'mfcc_6_k', 'mfcc_11_k', 'EnergyBurst_k', 'tot_articulation_p', 'shimmer_apq11_p', 'f2_max_p', 'mfcc_1_p', 'mfcc_10_p', 'mfcc_11_p', 'tot_articulation_t', 'mfcc_1_t', 'mfcc_3_t', 'mfcc_6_t', 'HFLFRatio_t']</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>5</v>
-      </c>
-      <c r="F16" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" t="n">
-        <v>8</v>
-      </c>
-      <c r="H16" t="n">
-        <v>5</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0.5882352941176471</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="N16" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="O16" t="n">
-        <v>0.8051948051948052</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>